<commit_message>
Ran parse_html.py for stories
</commit_message>
<xml_diff>
--- a/AllStories.xlsx
+++ b/AllStories.xlsx
@@ -20,7 +20,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="315">
+  <si>
+    <t xml:space="preserve">1 Bodystory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Clothesstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Family Membersstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Modes of Transportationstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Places in My Communitystory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Rooms in my housestory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Work Placesstory</t>
+  </si>
   <si>
     <t xml:space="preserve">Body</t>
   </si>
@@ -184,6 +205,24 @@
     <t xml:space="preserve">This is my family.</t>
   </si>
   <si>
+    <t xml:space="preserve">2 Ailmentsstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Colorsstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Describing story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Places I Gostory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Furniture in my housestory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Jobs in My Communitystory</t>
+  </si>
+  <si>
     <t xml:space="preserve">Flu</t>
   </si>
   <si>
@@ -337,12 +376,36 @@
     <t xml:space="preserve">In my kitchen, I have a rug.</t>
   </si>
   <si>
+    <t xml:space="preserve">2 Things I Needstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Settingsstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Job Dutiesstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Medicinestory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Sizesstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 School Yearsstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Signs in My Communitystory</t>
+  </si>
+  <si>
     <t xml:space="preserve">To Do List</t>
   </si>
   <si>
     <t xml:space="preserve">Rice</t>
   </si>
   <si>
+    <t xml:space="preserve">My Job</t>
+  </si>
+  <si>
     <t xml:space="preserve">Buying Medicine</t>
   </si>
   <si>
@@ -361,6 +424,9 @@
     <t xml:space="preserve">I turn the stove on.</t>
   </si>
   <si>
+    <t xml:space="preserve">My job is to grow food.</t>
+  </si>
+  <si>
     <t xml:space="preserve">My leg hurts.</t>
   </si>
   <si>
@@ -379,7 +445,7 @@
     <t xml:space="preserve">I turn the stove to medium.</t>
   </si>
   <si>
-    <t xml:space="preserve">My Job</t>
+    <t xml:space="preserve">My job is to count money.</t>
   </si>
   <si>
     <t xml:space="preserve">I don’t need cough syrup.</t>
@@ -400,7 +466,7 @@
     <t xml:space="preserve">I turn the stove to high.</t>
   </si>
   <si>
-    <t xml:space="preserve">My job is to grow food.</t>
+    <t xml:space="preserve">My job is to drive the bus.</t>
   </si>
   <si>
     <t xml:space="preserve">I don’t need cream.</t>
@@ -421,7 +487,7 @@
     <t xml:space="preserve">Oh no!</t>
   </si>
   <si>
-    <t xml:space="preserve">My job is to count money.</t>
+    <t xml:space="preserve">My job is to fix cars.</t>
   </si>
   <si>
     <t xml:space="preserve">I don’t need band aids.</t>
@@ -442,7 +508,7 @@
     <t xml:space="preserve">I turn the stove off.</t>
   </si>
   <si>
-    <t xml:space="preserve">My job is to drive the bus.</t>
+    <t xml:space="preserve">My job is to teach a class.</t>
   </si>
   <si>
     <t xml:space="preserve">I don’t need eye drops.</t>
@@ -463,7 +529,7 @@
     <t xml:space="preserve">I eat rice.</t>
   </si>
   <si>
-    <t xml:space="preserve">My job is to fix cars.</t>
+    <t xml:space="preserve">My job is to clean the room.</t>
   </si>
   <si>
     <t xml:space="preserve">I don’t need ointment.</t>
@@ -481,9 +547,6 @@
     <t xml:space="preserve">I go to the school.</t>
   </si>
   <si>
-    <t xml:space="preserve">My job is to teach a class.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The pants fit!</t>
   </si>
   <si>
@@ -496,9 +559,6 @@
     <t xml:space="preserve">I take a class.</t>
   </si>
   <si>
-    <t xml:space="preserve">My job is to clean the room.</t>
-  </si>
-  <si>
     <t xml:space="preserve">I need aspirin.</t>
   </si>
   <si>
@@ -508,6 +568,24 @@
     <t xml:space="preserve">Some children are in college.</t>
   </si>
   <si>
+    <t xml:space="preserve">3 Traffic Signsstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Directionsstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Problems in my apartmentstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Appointmentstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 School Suppliesstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Emergency Workersstory</t>
+  </si>
+  <si>
     <t xml:space="preserve">I Read the Signs</t>
   </si>
   <si>
@@ -664,6 +742,27 @@
     <t xml:space="preserve">She is ready for school.</t>
   </si>
   <si>
+    <t xml:space="preserve">5 Taking the Busstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Weatherstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Emergencystory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 City State Country_45story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Shoppingstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Housing Adsstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 Interviews and Applicationsstory</t>
+  </si>
+  <si>
     <t xml:space="preserve">The City Bus</t>
   </si>
   <si>
@@ -838,10 +937,13 @@
     <t xml:space="preserve">I say, “Thank you.”</t>
   </si>
   <si>
-    <t xml:space="preserve">HAP School</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I go to HAP school.</t>
+    <t xml:space="preserve">5 Teacher Directionsstory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I go to school.</t>
   </si>
   <si>
     <t xml:space="preserve">I look at the teacher.</t>
@@ -877,6 +979,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -936,8 +1039,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -958,994 +1065,1111 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M4" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="K5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="M5" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="K6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="M6" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="0" t="s">
+      <c r="I7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="0" t="s">
+      <c r="K7" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="M7" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K11" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M11" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>59</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K13" s="0" t="s">
+      <c r="I13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="0" t="s">
+      <c r="K13" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="M13" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K14" s="0" t="s">
+      <c r="I14" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M14" s="0" t="s">
+      <c r="K14" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="M14" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="I15" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M15" s="0" t="s">
+      <c r="K15" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="M15" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K16" s="0" t="s">
+      <c r="I16" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M16" s="0" t="s">
+      <c r="K16" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="M16" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K17" s="0" t="s">
+      <c r="I17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M17" s="0" t="s">
+      <c r="K17" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="M17" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="I18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="M18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="I18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="M19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="C19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K20" s="0" t="s">
-        <v>104</v>
+      <c r="C20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I22" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>106</v>
+      <c r="K22" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>112</v>
-      </c>
+      <c r="K23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="G24" s="0" t="s">
-        <v>116</v>
-      </c>
       <c r="I24" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I25" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="K25" s="0" t="s">
+      <c r="I25" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="M25" s="0" t="s">
+      <c r="K25" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="M25" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="C26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="G26" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="K26" s="0" t="s">
+      <c r="I26" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="M26" s="0" t="s">
+      <c r="K26" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="M26" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="G27" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="K27" s="0" t="s">
+      <c r="I27" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="M27" s="0" t="s">
+      <c r="K27" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="M27" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="C28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="G28" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="K28" s="0" t="s">
+      <c r="I28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M28" s="0" t="s">
+      <c r="K28" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="M28" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="C29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="I29" s="0" t="s">
+      <c r="G29" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="M29" s="0" t="s">
+      <c r="I29" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="K29" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="G30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="M30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>158</v>
       </c>
+      <c r="G30" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>161</v>
+      <c r="A31" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G33" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="K33" s="0" t="s">
-        <v>164</v>
+      <c r="A33" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="K35" s="0" t="s">
-        <v>176</v>
+      <c r="A34" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>179</v>
-      </c>
       <c r="G36" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="G37" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="I37" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="K37" s="0" t="s">
+      <c r="G37" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="I37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="E38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="G38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="I38" s="0" t="s">
+      <c r="E38" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="K38" s="0" t="s">
+      <c r="G38" s="1" t="s">
         <v>194</v>
       </c>
+      <c r="I38" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="E39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="G39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="I39" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="K39" s="0" t="s">
+      <c r="G39" s="1" t="s">
         <v>200</v>
       </c>
+      <c r="I39" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="E40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="G40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="I40" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="K40" s="0" t="s">
+      <c r="E40" s="1" t="s">
         <v>205</v>
       </c>
+      <c r="G40" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>206</v>
-      </c>
-      <c r="C41" s="0" t="s">
+      <c r="A41" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E41" s="0" t="s">
-        <v>208</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="K41" s="0" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>212</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="E44" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="G44" s="0" t="s">
-        <v>216</v>
-      </c>
-      <c r="I44" s="0" t="s">
-        <v>217</v>
-      </c>
-      <c r="K44" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="M44" s="0" t="s">
-        <v>219</v>
+      <c r="K44" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>220</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>221</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="I45" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="K45" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="M45" s="0" t="s">
-        <v>226</v>
+      <c r="A45" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>227</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>228</v>
-      </c>
-      <c r="E46" s="0" t="s">
-        <v>229</v>
-      </c>
-      <c r="G46" s="0" t="s">
-        <v>230</v>
-      </c>
-      <c r="I46" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="K46" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="M46" s="0" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>234</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="E47" s="0" t="s">
-        <v>236</v>
-      </c>
-      <c r="G47" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="I47" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="K47" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="M47" s="0" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="C48" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="E48" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="G48" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="G48" s="0" t="s">
+      <c r="I48" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="I48" s="0" t="s">
+      <c r="K48" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="K48" s="0" t="s">
+      <c r="M48" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="M48" s="0" t="s">
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="E49" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="I49" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="G49" s="0" t="s">
+      <c r="K49" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="I49" s="0" t="s">
+      <c r="M49" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="K49" s="0" t="s">
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="M49" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="E50" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="G50" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E50" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="G50" s="0" t="s">
+      <c r="I50" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="I50" s="0" t="s">
+      <c r="K50" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="K50" s="0" t="s">
+      <c r="M50" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="M50" s="0" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="E51" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="G51" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="I51" s="0" t="s">
+      <c r="I51" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="K51" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="M51" s="0" t="s">
+      <c r="K51" s="1" t="s">
         <v>265</v>
       </c>
+      <c r="M51" s="1" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="C52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="I52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="K52" s="0" t="s">
+      <c r="E52" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="M52" s="0" t="s">
+      <c r="G52" s="1" t="s">
         <v>270</v>
       </c>
+      <c r="I52" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>271</v>
+      <c r="A53" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>175</v>
+      <c r="A54" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>272</v>
+      <c r="A56" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>273</v>
+      <c r="A57" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>274</v>
+      <c r="A58" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>276</v>
+      <c r="A59" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>277</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>278</v>
+      <c r="A62" s="1" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>279</v>
+      <c r="A63" s="1" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>280</v>
+      <c r="A64" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>

</xml_diff>